<commit_message>
Added more advanced tests
</commit_message>
<xml_diff>
--- a/test/input-files/example.xlsx
+++ b/test/input-files/example.xlsx
@@ -377,21 +377,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
+      <c r="D1">
+        <f>18+24</f>
+        <v>42</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>